<commit_message>
Added Sitemap parsing, corrected configuration files, modified items file path
</commit_message>
<xml_diff>
--- a/doc/OpenHAB_configuration.xlsx
+++ b/doc/OpenHAB_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="180">
   <si>
     <t>item desc</t>
   </si>
@@ -377,24 +377,6 @@
     <t>Frame label</t>
   </si>
   <si>
-    <t>Item_label</t>
-  </si>
-  <si>
-    <t>mappings</t>
-  </si>
-  <si>
-    <t>icon</t>
-  </si>
-  <si>
-    <t>minValue</t>
-  </si>
-  <si>
-    <t>maxValue</t>
-  </si>
-  <si>
-    <t>step</t>
-  </si>
-  <si>
     <t>Setpoint</t>
   </si>
   <si>
@@ -573,6 +555,27 @@
   </si>
   <si>
     <t>budzik</t>
+  </si>
+  <si>
+    <t>Item name</t>
+  </si>
+  <si>
+    <t>Mappings</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>MinValue</t>
+  </si>
+  <si>
+    <t>MaxValue</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Item label</t>
   </si>
 </sst>
 </file>
@@ -901,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,10 +952,10 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F2" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -966,7 +969,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,7 +983,7 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1027,7 +1030,7 @@
         <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -1044,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -1061,7 +1064,7 @@
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -1125,7 +1128,7 @@
         <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -1145,7 +1148,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
@@ -1165,7 +1168,7 @@
         <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1185,7 +1188,7 @@
         <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -1205,7 +1208,7 @@
         <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1225,7 +1228,7 @@
         <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
@@ -1245,7 +1248,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
@@ -1320,7 +1323,7 @@
         <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
@@ -1340,7 +1343,7 @@
         <v>87</v>
       </c>
       <c r="E32" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F32" t="s">
         <v>9</v>
@@ -1371,7 +1374,7 @@
         <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F34" t="s">
         <v>9</v>
@@ -1388,7 +1391,7 @@
         <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
         <v>9</v>
@@ -1534,7 +1537,7 @@
         <v>27</v>
       </c>
       <c r="E50" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
@@ -1551,7 +1554,7 @@
         <v>28</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F51" t="s">
         <v>10</v>
@@ -1579,7 +1582,7 @@
         <v>108</v>
       </c>
       <c r="E53" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
@@ -1596,7 +1599,7 @@
         <v>109</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F54" t="s">
         <v>10</v>
@@ -1613,7 +1616,7 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="F55" t="s">
         <v>10</v>
@@ -1736,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,28 +1768,28 @@
         <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>173</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>179</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="G1" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="H1" t="s">
-        <v>116</v>
+        <v>176</v>
       </c>
       <c r="I1" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="J1" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="K1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1794,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -1902,7 +1905,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -1911,10 +1914,10 @@
         <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="F9" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="K9" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D9)&gt;0</f>
@@ -1926,10 +1929,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
         <v>76</v>
@@ -1944,7 +1947,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
         <v>73</v>
@@ -1959,7 +1962,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D12" t="s">
         <v>74</v>
@@ -1989,19 +1992,19 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
         <v>104</v>
       </c>
       <c r="E14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K14" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D14)&gt;0</f>
@@ -2010,13 +2013,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
         <v>102</v>
@@ -2037,10 +2040,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D16" t="s">
         <v>103</v>
@@ -2061,7 +2064,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2076,10 +2079,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -2097,19 +2100,19 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G19" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K19" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D19)&gt;0</f>
@@ -2118,13 +2121,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
@@ -2145,10 +2148,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
         <v>33</v>
@@ -2169,7 +2172,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2184,7 +2187,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -2199,7 +2202,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2214,16 +2217,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F25" t="str">
         <f>"@Stacje"</f>
@@ -2239,19 +2242,19 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K26" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D26)&gt;0</f>
@@ -2260,13 +2263,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
@@ -2287,10 +2290,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D28" t="s">
         <v>22</v>
@@ -2311,7 +2314,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
         <v>19</v>
@@ -2341,16 +2344,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F31" t="str">
         <f>"@Stacje"</f>
@@ -2366,19 +2369,19 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
         <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F32" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="K32" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D32)&gt;0</f>
@@ -2390,16 +2393,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>79</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F33" t="str">
         <f>"@Stacje"</f>
@@ -2415,19 +2418,19 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
         <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F34" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="K34" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D34)&gt;0</f>
@@ -2439,7 +2442,7 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
         <v>19</v>
@@ -2463,7 +2466,7 @@
         <v>63</v>
       </c>
       <c r="F36" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K36" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D36)&gt;0</f>
@@ -2481,7 +2484,7 @@
         <v>64</v>
       </c>
       <c r="F37" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K37" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D37)&gt;0</f>
@@ -2508,7 +2511,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
         <v>66</v>
@@ -2561,7 +2564,7 @@
         <v>110</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2569,7 +2572,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2577,7 +2580,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2585,7 +2588,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2601,7 +2604,7 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2609,27 +2612,27 @@
         <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2652,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2660,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2668,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2676,7 +2679,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2684,7 +2687,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,7 +2695,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2700,7 +2703,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2708,7 +2711,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OpenHAB configuration - modified Sheet headings
</commit_message>
<xml_diff>
--- a/doc/OpenHAB_configuration.xlsx
+++ b/doc/OpenHAB_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -36,28 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="180">
-  <si>
-    <t>item desc</t>
-  </si>
-  <si>
-    <t>item type</t>
-  </si>
-  <si>
-    <t>item name</t>
-  </si>
-  <si>
-    <t>labeltext</t>
-  </si>
-  <si>
-    <t>iconname</t>
-  </si>
-  <si>
-    <t>group1, group2, ...</t>
-  </si>
-  <si>
-    <t>bindingconfig</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="178">
   <si>
     <t>Group name</t>
   </si>
@@ -576,6 +555,21 @@
   </si>
   <si>
     <t>Item label</t>
+  </si>
+  <si>
+    <t>Item desc</t>
+  </si>
+  <si>
+    <t>Labeltext</t>
+  </si>
+  <si>
+    <t>Iconname</t>
+  </si>
+  <si>
+    <t>Group1, Group2, ...</t>
+  </si>
+  <si>
+    <t>Bindingconfig</t>
   </si>
 </sst>
 </file>
@@ -905,7 +899,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,706 +914,706 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>174</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>175</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
         <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>164</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="s">
         <v>48</v>
-      </c>
-      <c r="E18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
         <v>49</v>
-      </c>
-      <c r="E19" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>158</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" t="s">
         <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" t="s">
         <v>51</v>
-      </c>
-      <c r="E21" t="s">
-        <v>166</v>
-      </c>
-      <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
         <v>52</v>
-      </c>
-      <c r="E22" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
         <v>53</v>
-      </c>
-      <c r="E23" t="s">
-        <v>168</v>
-      </c>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" t="s">
         <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="G29" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E31" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="F34" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F35" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F36" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F37" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G46" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G47" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G48" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E50" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E51" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D53" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E53" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E54" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E55" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1655,79 +1649,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1739,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1759,37 +1753,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="I1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="J1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1797,13 +1791,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K2" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D2)&gt;0</f>
@@ -1815,10 +1809,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="K3" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D3)&gt;0</f>
@@ -1830,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="K4" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D4)&gt;0</f>
@@ -1845,10 +1839,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="K5" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D5)&gt;0</f>
@@ -1860,10 +1854,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="K6" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D6)&gt;0</f>
@@ -1875,10 +1869,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="K7" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D7)&gt;0</f>
@@ -1890,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="K8" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D8)&gt;0</f>
@@ -1905,19 +1899,19 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="K9" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D9)&gt;0</f>
@@ -1929,13 +1923,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K10" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D10)&gt;0</f>
@@ -1947,10 +1941,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="K11" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D11)&gt;0</f>
@@ -1962,10 +1956,10 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K12" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D12)&gt;0</f>
@@ -1977,10 +1971,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="K13" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D13)&gt;0</f>
@@ -1992,19 +1986,19 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K14" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D14)&gt;0</f>
@@ -2013,16 +2007,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2040,13 +2034,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2064,13 +2058,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K17" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D17)&gt;0</f>
@@ -2079,16 +2073,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K18" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D18)&gt;0</f>
@@ -2100,19 +2094,19 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G19" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="K19" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D19)&gt;0</f>
@@ -2121,16 +2115,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2148,13 +2142,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2172,13 +2166,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K22" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D22)&gt;0</f>
@@ -2187,13 +2181,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="K23" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D23)&gt;0</f>
@@ -2202,13 +2196,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="K24" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D24)&gt;0</f>
@@ -2217,16 +2211,16 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F25" t="str">
         <f>"@Stacje"</f>
@@ -2242,19 +2236,19 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="K26" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D26)&gt;0</f>
@@ -2263,16 +2257,16 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2290,13 +2284,13 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -2314,13 +2308,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K29" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D29)&gt;0</f>
@@ -2329,13 +2323,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
         <v>19</v>
-      </c>
-      <c r="D30" t="s">
-        <v>26</v>
       </c>
       <c r="K30" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D30)&gt;0</f>
@@ -2344,16 +2338,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E31" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F31" t="str">
         <f>"@Stacje"</f>
@@ -2369,19 +2363,19 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F32" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K32" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D32)&gt;0</f>
@@ -2393,16 +2387,16 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F33" t="str">
         <f>"@Stacje"</f>
@@ -2418,19 +2412,19 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F34" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K34" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D34)&gt;0</f>
@@ -2442,13 +2436,13 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="K35" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D35)&gt;0</f>
@@ -2460,13 +2454,13 @@
         <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F36" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K36" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D36)&gt;0</f>
@@ -2478,13 +2472,13 @@
         <v>10</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K37" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D37)&gt;0</f>
@@ -2496,10 +2490,10 @@
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="K38" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D38)&gt;0</f>
@@ -2511,10 +2505,10 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D39" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="K39" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D39)&gt;0</f>
@@ -2561,78 +2555,78 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2644,7 +2638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2655,7 +2649,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2663,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2671,7 +2665,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2679,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2687,7 +2681,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2695,7 +2689,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2703,7 +2697,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,7 +2705,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the Sitemaps sheet structure
</commit_message>
<xml_diff>
--- a/doc/OpenHAB_configuration.xlsx
+++ b/doc/OpenHAB_configuration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="178">
   <si>
     <t>Group name</t>
   </si>
@@ -612,7 +612,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1618,7 +1646,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
@@ -1731,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,15 +1821,9 @@
       <c r="B2" t="s">
         <v>151</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
       <c r="K2" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D2)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1812,7 +1834,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D3)&gt;0</f>
@@ -1827,7 +1849,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D4)&gt;0</f>
@@ -1842,7 +1864,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D5)&gt;0</f>
@@ -1857,7 +1879,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D6)&gt;0</f>
@@ -1872,7 +1894,7 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K7" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D7)&gt;0</f>
@@ -1887,7 +1909,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K8" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D8)&gt;0</f>
@@ -1896,22 +1918,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>116</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="K9" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D9)&gt;0</f>
@@ -1920,31 +1933,31 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" t="s">
-        <v>108</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="K10" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D10)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>89</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>118</v>
       </c>
       <c r="K11" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D11)&gt;0</f>
@@ -1955,15 +1968,12 @@
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
+      <c r="B12" t="s">
+        <v>119</v>
       </c>
       <c r="K12" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D12)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1971,10 +1981,10 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D13)&gt;0</f>
@@ -1983,22 +1993,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
-      </c>
-      <c r="B14" t="s">
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" t="s">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="K14" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D14)&gt;0</f>
@@ -2006,26 +2007,14 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
+      <c r="A15">
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>23</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="K15" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D15)&gt;0</f>
@@ -2033,23 +2022,14 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>123</v>
+      <c r="A16">
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>55</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="K16" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D16)&gt;0</f>
@@ -2057,32 +2037,32 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>98</v>
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>120</v>
       </c>
       <c r="K17" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D17)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" t="s">
-        <v>126</v>
+      <c r="A18">
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
       </c>
       <c r="K18" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D18)&gt;0</f>
@@ -2090,41 +2070,26 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>5</v>
+      <c r="A19" t="s">
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>127</v>
-      </c>
-      <c r="C19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K19" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D19)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>130</v>
-      </c>
-      <c r="B20" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
         <v>106</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2142,22 +2107,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
         <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K21" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D21)&gt;0</f>
@@ -2166,13 +2131,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="K22" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D22)&gt;0</f>
@@ -2181,28 +2146,25 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
+        <v>125</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
       </c>
       <c r="K23" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D23)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="K24" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D24)&gt;0</f>
@@ -2210,42 +2172,29 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C25" t="s">
-        <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" t="str">
-        <f>"@Stacje"</f>
-        <v>@Stacje</v>
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
       </c>
       <c r="K25" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D25)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
+        <v>5</v>
       </c>
       <c r="C26" t="s">
         <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E26" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G26" t="s">
         <v>129</v>
@@ -2257,49 +2206,34 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
         <v>131</v>
       </c>
-      <c r="C27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>23</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
       <c r="K27" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D27)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
         <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="J28">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K28" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D28)&gt;0</f>
@@ -2308,13 +2242,22 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>50</v>
+      </c>
+      <c r="J29">
+        <v>10</v>
       </c>
       <c r="K29" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D29)&gt;0</f>
@@ -2323,13 +2266,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="K30" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D30)&gt;0</f>
@@ -2338,20 +2281,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>132</v>
-      </c>
-      <c r="F31" t="str">
-        <f>"@Stacje"</f>
-        <v>@Stacje</v>
+        <v>29</v>
       </c>
       <c r="K31" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D31)&gt;0</f>
@@ -2359,23 +2295,14 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>7</v>
-      </c>
-      <c r="B32" t="s">
-        <v>136</v>
+      <c r="A32" t="s">
+        <v>130</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>71</v>
-      </c>
-      <c r="E32" t="s">
-        <v>137</v>
-      </c>
-      <c r="F32" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="K32" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D32)&gt;0</f>
@@ -2383,17 +2310,14 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
+      <c r="A33" t="s">
+        <v>130</v>
       </c>
       <c r="C33" t="s">
         <v>107</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
         <v>132</v>
@@ -2409,40 +2333,31 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C34" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="K34" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D34)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>10</v>
-      </c>
-      <c r="B35" t="s">
-        <v>149</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>60</v>
+        <v>18</v>
+      </c>
+      <c r="E35" t="s">
+        <v>134</v>
+      </c>
+      <c r="G35" t="s">
+        <v>129</v>
       </c>
       <c r="K35" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D35)&gt;0</f>
@@ -2450,35 +2365,35 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" t="s">
-        <v>150</v>
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
       </c>
       <c r="K36" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D36)&gt;0</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>10</v>
+      <c r="A37" t="s">
+        <v>135</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>150</v>
+        <v>14</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>23</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
       </c>
       <c r="K37" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D37)&gt;0</f>
@@ -2486,14 +2401,23 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>50</v>
+      </c>
+      <c r="J38">
         <v>10</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>58</v>
       </c>
       <c r="K38" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D38)&gt;0</f>
@@ -2501,30 +2425,539 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>10</v>
+      <c r="A39" t="s">
+        <v>135</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="K39" t="b">
         <f>COUNTIF(Items!C$2:C$636, Sitemap!D39)&gt;0</f>
         <v>1</v>
       </c>
     </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="K40" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D40)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" t="str">
+        <f>"@Stacje"</f>
+        <v>@Stacje</v>
+      </c>
+      <c r="K41" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D41)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="K42" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D42)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" t="s">
+        <v>138</v>
+      </c>
+      <c r="K43" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D43)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>145</v>
+      </c>
+      <c r="K44" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D44)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>8</v>
+      </c>
+      <c r="C45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" t="str">
+        <f>"@Stacje"</f>
+        <v>@Stacje</v>
+      </c>
+      <c r="K45" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D45)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="K46" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D46)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F47" t="s">
+        <v>148</v>
+      </c>
+      <c r="K47" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D47)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>149</v>
+      </c>
+      <c r="K48" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D48)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+      <c r="K49" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D49)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" t="s">
+        <v>150</v>
+      </c>
+      <c r="K50" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D50)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" t="s">
+        <v>150</v>
+      </c>
+      <c r="K51" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D51)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>10</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="K52" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D52)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>59</v>
+      </c>
+      <c r="K53" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D53)&gt;0</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K54" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D54)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K55" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D55)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K56" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D56)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K57" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D57)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K58" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D58)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K59" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D59)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K60" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D60)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K61" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D61)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K62" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D62)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K63" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D63)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K64" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D64)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D65)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D66)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D67)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D68)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D69)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D70)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D71)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K72" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D72)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K73" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D73)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K74" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D74)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K75" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D75)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K76" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D76)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K77" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D77)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K78" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D78)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K79" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D79)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K80" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D80)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K81" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D81)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K82" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D82)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K83" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D83)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K84" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D84)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K85" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D85)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K86" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D86)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K87" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D87)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K88" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D88)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K89" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D89)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K90" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D90)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K91" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D91)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K92" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D92)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K93" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D93)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K94" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D94)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K95" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D95)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K96" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D96)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K97" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D97)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K98" t="b">
+        <f>COUNTIF(Items!C$2:C$636, Sitemap!D98)&gt;0</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:K98">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$K$2="FALSE"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C9 C11 C13:C16 C18 C20:C22 C24 C26 C28:C33 C35 C37:C41 C43 C45 C49:C1048576 C47">
       <formula1>Item_type_sitemap</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D9 D11 D13:D16 D18 D20:D22 D24 D26 D28:D33 D35 D37:D41 D43 D45 D49:D1048576 D47">
       <formula1>Item_names</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2545,7 +2978,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,7 +3071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>